<commit_message>
Se agrega el caso en el que k sea un funcion de t y el caso en el que y esté elevado a la n-potencia
</commit_message>
<xml_diff>
--- a/output/euleredo.xlsx
+++ b/output/euleredo.xlsx
@@ -398,394 +398,394 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="B3">
-        <v>2.3</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="B4">
-        <v>2.6399999999999997</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>0.30000000000000004</v>
+        <v>0.75</v>
       </c>
       <c r="B5">
-        <v>3.0279999999999996</v>
+        <v>5.125</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>3.4735999999999994</v>
+        <v>7.0625</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="B7">
-        <v>3.9883199999999994</v>
+        <v>9.84375</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>0.6</v>
+        <v>1.5</v>
       </c>
       <c r="B8">
-        <v>4.585983999999999</v>
+        <v>13.890625</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>0.7</v>
+        <v>1.75</v>
       </c>
       <c r="B9">
-        <v>5.2831807999999985</v>
+        <v>19.8359375</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>0.7999999999999999</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>6.099816959999998</v>
+        <v>28.62890625</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>0.8999999999999999</v>
+        <v>2.25</v>
       </c>
       <c r="B11">
-        <v>7.059780351999998</v>
+        <v>41.693359375</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>0.9999999999999999</v>
+        <v>2.5</v>
       </c>
       <c r="B12">
-        <v>8.191736422399998</v>
+        <v>61.1650390625</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>1.0999999999999999</v>
+        <v>2.75</v>
       </c>
       <c r="B13">
-        <v>9.530083706879998</v>
+        <v>90.24755859375</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>1.2</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>11.116100448255997</v>
+        <v>133.746337890625</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>1.3</v>
+        <v>3.25</v>
       </c>
       <c r="B15">
-        <v>12.999320537907197</v>
+        <v>198.8695068359375</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>1.4000000000000001</v>
+        <v>3.5</v>
       </c>
       <c r="B16">
-        <v>15.239184645488637</v>
+        <v>296.42926025390625</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>1.5000000000000002</v>
+        <v>3.75</v>
       </c>
       <c r="B17">
-        <v>17.907021574586363</v>
+        <v>442.6438903808594</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>1.6000000000000003</v>
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>21.088425889503636</v>
+        <v>661.8408355712891</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>1.7000000000000004</v>
+        <v>4.25</v>
       </c>
       <c r="B19">
-        <v>24.886111067404364</v>
+        <v>990.5112533569336</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>1.8000000000000005</v>
+        <v>4.5</v>
       </c>
       <c r="B20">
-        <v>29.423333280885238</v>
+        <v>1483.3918800354004</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>1.9000000000000006</v>
+        <v>4.75</v>
       </c>
       <c r="B21">
-        <v>34.84799993706228</v>
+        <v>2222.5878200531006</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>2.0000000000000004</v>
+        <v>5</v>
       </c>
       <c r="B22">
-        <v>41.337599924474745</v>
+        <v>3331.256730079651</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>2.1000000000000005</v>
+        <v>5.25</v>
       </c>
       <c r="B23">
-        <v>49.10511990936969</v>
+        <v>4994.135095119476</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2.2000000000000006</v>
+        <v>5.5</v>
       </c>
       <c r="B24">
-        <v>58.40614389124363</v>
+        <v>7488.3276426792145</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>2.3000000000000007</v>
+        <v>5.75</v>
       </c>
       <c r="B25">
-        <v>69.54737266949236</v>
+        <v>11229.491464018822</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>2.400000000000001</v>
+        <v>6</v>
       </c>
       <c r="B26">
-        <v>82.89684720339083</v>
+        <v>16841.112196028233</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>2.500000000000001</v>
+        <v>6.25</v>
       </c>
       <c r="B27">
-        <v>98.896216644069</v>
+        <v>25258.41829404235</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>2.600000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="B28">
-        <v>118.0754599728828</v>
+        <v>37884.25244106352</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>2.700000000000001</v>
+        <v>6.75</v>
       </c>
       <c r="B29">
-        <v>141.07055196745935</v>
+        <v>56822.878661595285</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>2.800000000000001</v>
+        <v>7</v>
       </c>
       <c r="B30">
-        <v>168.64466236095123</v>
+        <v>85230.69299239293</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>2.9000000000000012</v>
+        <v>7.25</v>
       </c>
       <c r="B31">
-        <v>201.71359483314149</v>
+        <v>127842.28948858939</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>3.0000000000000013</v>
+        <v>7.5</v>
       </c>
       <c r="B32">
-        <v>241.37631379976978</v>
+        <v>191759.5592328841</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>3.1000000000000014</v>
+        <v>7.75</v>
       </c>
       <c r="B33">
-        <v>288.9515765597237</v>
+        <v>287635.33884932613</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>3.2000000000000015</v>
+        <v>8</v>
       </c>
       <c r="B34">
-        <v>346.02189187166846</v>
+        <v>431448.8832739892</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>3.3000000000000016</v>
+        <v>8.25</v>
       </c>
       <c r="B35">
-        <v>414.48627024600216</v>
+        <v>647169.0749109838</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>3.4000000000000017</v>
+        <v>8.5</v>
       </c>
       <c r="B36">
-        <v>496.6235242952026</v>
+        <v>970749.2373664756</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>3.5000000000000018</v>
+        <v>8.75</v>
       </c>
       <c r="B37">
-        <v>595.1682291542431</v>
+        <v>1456119.3560497134</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>3.600000000000002</v>
+        <v>9</v>
       </c>
       <c r="B38">
-        <v>713.4018749850918</v>
+        <v>2184174.40907457</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>3.700000000000002</v>
+        <v>9.25</v>
       </c>
       <c r="B39">
-        <v>855.2622499821102</v>
+        <v>3276256.863611855</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>3.800000000000002</v>
+        <v>9.5</v>
       </c>
       <c r="B40">
-        <v>1025.4746999785323</v>
+        <v>4914380.420417783</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>3.900000000000002</v>
+        <v>9.75</v>
       </c>
       <c r="B41">
-        <v>1229.7096399742388</v>
+        <v>7371565.630626675</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>4.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="B42">
-        <v>1474.7715679690866</v>
+        <v>11057343.320940012</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>4.100000000000001</v>
+        <v>10.25</v>
       </c>
       <c r="B43">
-        <v>1768.825881562904</v>
+        <v>16586009.73141002</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>4.200000000000001</v>
+        <v>10.5</v>
       </c>
       <c r="B44">
-        <v>2121.6710578754846</v>
+        <v>24879009.22211503</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>4.300000000000001</v>
+        <v>10.75</v>
       </c>
       <c r="B45">
-        <v>2545.0652694505816</v>
+        <v>37318508.333172545</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>4.4</v>
+        <v>11</v>
       </c>
       <c r="B46">
-        <v>3053.1183233406978</v>
+        <v>55977756.87475882</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>4.5</v>
+        <v>11.25</v>
       </c>
       <c r="B47">
-        <v>3662.7619880088373</v>
+        <v>83966629.56213823</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>4.6</v>
+        <v>11.5</v>
       </c>
       <c r="B48">
-        <v>4394.314385610605</v>
+        <v>125949938.46820734</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>4.699999999999999</v>
+        <v>11.75</v>
       </c>
       <c r="B49">
-        <v>5272.157262732726</v>
+        <v>188924901.702311</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>4.799999999999999</v>
+        <v>12</v>
       </c>
       <c r="B50">
-        <v>6325.548715279271</v>
+        <v>283387346.4284665</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>4.899999999999999</v>
+        <v>12.25</v>
       </c>
       <c r="B51">
-        <v>7589.5984583351255</v>
+        <v>425081013.3926997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>